<commit_message>
docs: decompose user journey into stories and enablers
</commit_message>
<xml_diff>
--- a/docs/User_Story_Mapping_and_Decomposition.xlsx
+++ b/docs/User_Story_Mapping_and_Decomposition.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramos\Desktop\EMSS20252026\ptsd_protocol\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E76B40-CC49-4ABA-BEC9-518AE9ECD697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49A8ADC-16C3-41A5-8DD4-89FFB4841F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Functions per Step" sheetId="1" r:id="rId1"/>
+    <sheet name="Features from steps" sheetId="1" r:id="rId1"/>
+    <sheet name="Initial US from features" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="169">
   <si>
     <t>User Journey</t>
   </si>
@@ -46,9 +47,6 @@
     <t>5.2 Add device to device map</t>
   </si>
   <si>
-    <t>5.3 Load basic device profile</t>
-  </si>
-  <si>
     <t>6.3 Allow advanced security view</t>
   </si>
   <si>
@@ -91,9 +89,6 @@
     <t>3.4 Loading spinner</t>
   </si>
   <si>
-    <t>5.4 Load advanced device profile</t>
-  </si>
-  <si>
     <t>5.3 Show current status</t>
   </si>
   <si>
@@ -145,14 +140,498 @@
     <t>Feature 5</t>
   </si>
   <si>
-    <t>edsrdrefreswfers</t>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>User Story</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria</t>
+  </si>
+  <si>
+    <t>US1.1</t>
+  </si>
+  <si>
+    <t>As a user, I want the device to have a QR code so that I can scan it easily.</t>
+  </si>
+  <si>
+    <t>Given the user unpacks the device
+When they look at it
+Then a QR code is visible and scannable</t>
+  </si>
+  <si>
+    <t>US1.2</t>
+  </si>
+  <si>
+    <t>As a user, I want an instruction manual so that I know how to begin onboarding.</t>
+  </si>
+  <si>
+    <t>Given the device is unpacked
+When the user reads the manual
+Then steps direct them to the app and QR code</t>
+  </si>
+  <si>
+    <t>US2.1</t>
+  </si>
+  <si>
+    <t>As a user, I want a visible app icon so that I can open the HomeGuard app easily.</t>
+  </si>
+  <si>
+    <t>Given the app is installed
+When the user views the home screen
+Then the icon is visible and tappable</t>
+  </si>
+  <si>
+    <t>US2.2</t>
+  </si>
+  <si>
+    <t>US2.3</t>
+  </si>
+  <si>
+    <t>As a user, I want an Add Device button so that I can start onboarding quickly.</t>
+  </si>
+  <si>
+    <t>Given the user is on the home screen
+When they click Add Device
+Then onboarding starts</t>
+  </si>
+  <si>
+    <t>US3.1</t>
+  </si>
+  <si>
+    <t>As a user, I want the camera scanner to open so that I can scan the QR code.</t>
+  </si>
+  <si>
+    <t>US3.2</t>
+  </si>
+  <si>
+    <t>As a user, I want QR detection so that onboarding continues quickly.</t>
+  </si>
+  <si>
+    <t>US3.3</t>
+  </si>
+  <si>
+    <t>As a user, I want confirmation of successful scan so that I know to continue.</t>
+  </si>
+  <si>
+    <t>US3.4</t>
+  </si>
+  <si>
+    <t>Given pairing begins
+When key exchange runs
+Then no input is needed</t>
+  </si>
+  <si>
+    <t>US5.1</t>
+  </si>
+  <si>
+    <t>US5.2</t>
+  </si>
+  <si>
+    <t>As a user, I want the device added to the map so that I see it in my network.</t>
+  </si>
+  <si>
+    <t>Given device connected
+When map refreshes
+Then device appears</t>
+  </si>
+  <si>
+    <t>US5.3</t>
+  </si>
+  <si>
+    <t>As a user, I want basic info so that I can recognize the device.</t>
+  </si>
+  <si>
+    <t>US6.1</t>
+  </si>
+  <si>
+    <t>US6.2</t>
+  </si>
+  <si>
+    <t>As a user, I want secure defaults so that my device is protected fast.</t>
+  </si>
+  <si>
+    <t>Given recommendation shown
+When user taps secure defaults
+Then settings apply</t>
+  </si>
+  <si>
+    <t>US6.3</t>
+  </si>
+  <si>
+    <t>As a user, I want advanced security options so that I can customize behavior.</t>
+  </si>
+  <si>
+    <t>Given advanced view selected
+When advanced settings open
+Then user can modify permissions</t>
+  </si>
+  <si>
+    <t>US7.1</t>
+  </si>
+  <si>
+    <t>US7.2</t>
+  </si>
+  <si>
+    <t>US7.3</t>
+  </si>
+  <si>
+    <t>US7.4</t>
+  </si>
+  <si>
+    <t>As a user, I want a loading spinner so that I know the scan is being processes and I am not impatient.</t>
+  </si>
+  <si>
+    <t>Given scanning is attempted
+When QR information is being processed
+Then the loading spinner is visible</t>
+  </si>
+  <si>
+    <t>Given QR scan succeeded
+When pairing starts
+Then key exchange begins
+Given pairing begins
+When key exchange runs
+Then no input is needed
+And data is safely processed</t>
+  </si>
+  <si>
+    <t>US2.4</t>
+  </si>
+  <si>
+    <t>As a user, I want to see the list of my devices so that I know which devices are connected with secure protocol.</t>
+  </si>
+  <si>
+    <t>Given the user has the HomeGuard application opened
+When the main screen is opened
+Then the device list is visible
+And the devices connected are shown</t>
+  </si>
+  <si>
+    <t>Given HomeGuard application is opened
+When the user looks at the bottom of any screen
+Then the bottom menu is visible
+Given HomeGuard application is opened
+When user clicks on any bottom menu item
+Then the connected screen open</t>
+  </si>
+  <si>
+    <t>As a user, I want a bottom menu so that I can navigate through the application screens.</t>
+  </si>
+  <si>
+    <t>US2.5</t>
+  </si>
+  <si>
+    <t>Given HomeGuard app is opened
+When add device button is clicked
+Then camera view opens</t>
+  </si>
+  <si>
+    <t>Given the camera is opened
+When the QR code is visible
+Then camera scans the QR code</t>
+  </si>
+  <si>
+    <t>Given the QR is scanned
+When it is successful
+Then confirmation appears
+And camera closes
+Given the QR is scanned
+When it is wrong
+Then window with information appears
+And camera closes</t>
+  </si>
+  <si>
+    <t>E4.1</t>
+  </si>
+  <si>
+    <t>E4.2</t>
+  </si>
+  <si>
+    <t>Given device onboarding is in process
+When the connection was established
+Then the success confirmation is displayed</t>
+  </si>
+  <si>
+    <t>As a user I want to see a confirmation in HomeGuard app so that I know my data was correctly encrypted and the connection is secure.</t>
+  </si>
+  <si>
+    <t>5.4 Load basic device profile</t>
+  </si>
+  <si>
+    <t>5.5 Load advanced device profile</t>
+  </si>
+  <si>
+    <t>Given Homeguard app is opened
+When a device is visible on the list
+Then the status is displayed</t>
+  </si>
+  <si>
+    <t>Given HomeGuard app opened
+When user clicks the device
+Then basic device information is displayed</t>
+  </si>
+  <si>
+    <t>US5.4</t>
+  </si>
+  <si>
+    <t>US5.5</t>
+  </si>
+  <si>
+    <t>Given HomeGuard app opened
+When user clicks the device
+Then basic device information is displayed
+And the advanced information is displayed below</t>
+  </si>
+  <si>
+    <t>As a user, I want advanced info so that I can analyze the device performance.</t>
+  </si>
+  <si>
+    <t>Load basic device profile</t>
+  </si>
+  <si>
+    <t>As a user, I want a security note so that I understand that my IoT network is secure.</t>
+  </si>
+  <si>
+    <t>Given device connected
+When device type recognized
+Then security note shows</t>
+  </si>
+  <si>
+    <t>Given the HomeGuard app is installed
+When the user opens the app
+Then the main screen appears</t>
+  </si>
+  <si>
+    <t>As a user, I want a main screen so that I can perform actions in HomeGuard app.</t>
+  </si>
+  <si>
+    <t>Given device in the list
+When I click connection button
+Then device status is updated</t>
+  </si>
+  <si>
+    <t>As a user I want to be able to manage device connection so that I can connect or disconnect based on my needs.</t>
+  </si>
+  <si>
+    <t>As a user I want to be able to see device connection status so that I know if I need to connect or disconnect.</t>
+  </si>
+  <si>
+    <t>Given HomeGuard app opened
+When device is on the list
+Then the connection status is shown</t>
+  </si>
+  <si>
+    <t>Given HomeGuard app opened
+And device is on the list
+When the user clicks the device
+Then there is a button to change security settings
+And advanced security settings are shown under basic security settings</t>
+  </si>
+  <si>
+    <t>As a user I want to have ability to change advanced security settings so that i can configure the device deeply to my needs.</t>
+  </si>
+  <si>
+    <t>As a user I want to have ability to change basic security settings so that i can configure the device to my needs.</t>
+  </si>
+  <si>
+    <t>Given HomeGuard app opened
+And device is on the list
+When the user clicks the device
+Then there is a button to change security settings
+And basic security settings are shown</t>
+  </si>
+  <si>
+    <t>E4.3</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Enabler</t>
+  </si>
+  <si>
+    <t>Story</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Device Firmware with Privacy-Tuned Smart Device Protocol</t>
+  </si>
+  <si>
+    <t>10.1 Import device bluetooth settings</t>
+  </si>
+  <si>
+    <t>10. Set up device bluetooth</t>
+  </si>
+  <si>
+    <t>11. Exchange protocol keys</t>
+  </si>
+  <si>
+    <t>12. Exchange data and establish secure connection</t>
+  </si>
+  <si>
+    <t>10.2 Set up beacon</t>
+  </si>
+  <si>
+    <t>10.4 Energy management protocol</t>
+  </si>
+  <si>
+    <t>11.1 Generate keys based on device ID</t>
+  </si>
+  <si>
+    <t>11.3 Receive session key</t>
+  </si>
+  <si>
+    <t>11.2 Send public keys to mobile phone application using bluetooth connection</t>
+  </si>
+  <si>
+    <t>11.5 Send different keys based on connection type</t>
+  </si>
+  <si>
+    <t>11.4 Differentiate keys between different connection types</t>
+  </si>
+  <si>
+    <t>12.1 Ensure keys exchange</t>
+  </si>
+  <si>
+    <t>12.2 Exchange handshake</t>
+  </si>
+  <si>
+    <t>12.4 Check for connection stability</t>
+  </si>
+  <si>
+    <t>12.5 Implement connection stability improvement algorithm</t>
+  </si>
+  <si>
+    <t>E10.1</t>
+  </si>
+  <si>
+    <t>E10.2</t>
+  </si>
+  <si>
+    <t>E10.3</t>
+  </si>
+  <si>
+    <t>E11.1</t>
+  </si>
+  <si>
+    <t>E12.1</t>
+  </si>
+  <si>
+    <t>E11.2</t>
+  </si>
+  <si>
+    <t>E11.3</t>
+  </si>
+  <si>
+    <t>E11.4</t>
+  </si>
+  <si>
+    <t>E11.5</t>
+  </si>
+  <si>
+    <t>E12.2</t>
+  </si>
+  <si>
+    <t>E12.3</t>
+  </si>
+  <si>
+    <t>E12.4</t>
+  </si>
+  <si>
+    <t>E10.4</t>
+  </si>
+  <si>
+    <t>As a developer, I want cryptographic exchange handled automatically so that I can create visual output to the user.</t>
+  </si>
+  <si>
+    <t>As a developer, I want pairing to run the key exchange so that I will be able to show the user that the device connects securely.</t>
+  </si>
+  <si>
+    <t>As a developer I want retry option so that pairing failures can be fixed.</t>
+  </si>
+  <si>
+    <t>Given pairing fails
+When error occurs
+Then it is retried</t>
+  </si>
+  <si>
+    <t>10.3 Connection to mobile phone HomeGuard app</t>
+  </si>
+  <si>
+    <t>Given device is ON
+When the firmware runs
+Then the device bluetooth module is running and firmware has control over it</t>
+  </si>
+  <si>
+    <t>Given device is ON
+When the firmware runs
+Then the device is listening for communication from the mobile app</t>
+  </si>
+  <si>
+    <t>Given the firmware running
+When the request from mobile app comes
+Then the bluetooth connection is established</t>
+  </si>
+  <si>
+    <t>Given established connection
+When data is not exchanged
+Then energy saving protocol is running</t>
+  </si>
+  <si>
+    <t>Given bluetooth connection established
+When data exchange is requested
+Then keys are generated</t>
+  </si>
+  <si>
+    <t>Given keys generated
+When data echange is requested
+Then the public key is exchanged with the HomeGuard app</t>
+  </si>
+  <si>
+    <t>Given connection established
+When public key is received by HomeGuard
+Then session key is sent by HomeGuard and validated by the device</t>
+  </si>
+  <si>
+    <t>Given a connection type different than bluetooth
+When a key is exchanged
+Then the keys are different as for the different connection needs</t>
+  </si>
+  <si>
+    <t>Given a connection type different than bluetooth
+When a key is generated
+Then the keys are different as for the different connection needs</t>
+  </si>
+  <si>
+    <t>Given the bluetooth connection established
+When the exchanged keys are correct
+Then the connection is set as secure</t>
+  </si>
+  <si>
+    <t>Given the bluetooth connection established
+When the connection is set as secure
+Then the handshake is exchanged between the device and HomeGuard app</t>
+  </si>
+  <si>
+    <t>Given the bluetooth connection established
+When the connection is set as secure
+Then the connection stability status is being calculated</t>
+  </si>
+  <si>
+    <t>Given the bluetooth connection established
+When the connection stability status is calculated
+And the status is below treshold
+Then the improvement algorithm is running</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,8 +667,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -220,8 +706,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -329,11 +827,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -349,11 +858,511 @@
     <xf numFmtId="16" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="31">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -671,19 +1680,48 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A21E0A7F-BB4F-4BDE-A642-52BFB87453A8}" name="Tabela2" displayName="Tabela2" ref="A1:H6" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A21E0A7F-BB4F-4BDE-A642-52BFB87453A8}" name="Tabela2" displayName="Tabela2" ref="A1:H6" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <autoFilter ref="A1:H6" xr:uid="{A21E0A7F-BB4F-4BDE-A642-52BFB87453A8}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{3D043F1F-14D1-443A-9E49-75C310A69C02}" name="User Journey" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{817A37F1-0EA8-4F05-B834-AB936B045108}" name="1. Unpack The Device" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{07C082F0-0E2F-4FE0-931A-30473110F396}" name="2. Open App" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{2A1A6FC2-F5EB-43B6-A97F-846B1A1D8951}" name="3. Scan QR Code" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{6D12A665-90DB-4074-A462-0CD37108336F}" name="4. Secure Pairing" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{1743114B-01C7-47B6-966F-79B2DC546BA2}" name="5. See Connection" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{101D4D22-33DD-474D-A0A9-84B029559DF3}" name="6. Security Note" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{8BB13731-E190-45A5-A805-DD42B4771B70}" name="7. Use Device" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{3D043F1F-14D1-443A-9E49-75C310A69C02}" name="User Journey" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{817A37F1-0EA8-4F05-B834-AB936B045108}" name="1. Unpack The Device" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{07C082F0-0E2F-4FE0-931A-30473110F396}" name="2. Open App" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{2A1A6FC2-F5EB-43B6-A97F-846B1A1D8951}" name="3. Scan QR Code" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{6D12A665-90DB-4074-A462-0CD37108336F}" name="4. Secure Pairing" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{1743114B-01C7-47B6-966F-79B2DC546BA2}" name="5. See Connection" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{101D4D22-33DD-474D-A0A9-84B029559DF3}" name="6. Security Note" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{8BB13731-E190-45A5-A805-DD42B4771B70}" name="7. Use Device" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D0BA2CA0-54DF-49BE-881D-C4408A2DE1C0}" name="Tabela3" displayName="Tabela3" ref="A15:D20" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="16" tableBorderDxfId="17" totalsRowBorderDxfId="15">
+  <autoFilter ref="A15:D20" xr:uid="{D0BA2CA0-54DF-49BE-881D-C4408A2DE1C0}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{1230F03C-C2EB-45F1-B9A1-9AD74F5EC7A2}" name="Device Firmware with Privacy-Tuned Smart Device Protocol" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{F3A10773-0F0A-4C06-8A63-E52FC4019413}" name="10. Set up device bluetooth" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{55E1B1AC-0A6D-43B9-B218-8352877C9259}" name="11. Exchange protocol keys"/>
+    <tableColumn id="4" xr3:uid="{8EAE05D1-8B9C-497F-A5A7-A6A612CAEA2F}" name="12. Exchange data and establish secure connection"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FDB3D34F-B875-4993-9583-517C7A228CFA}" name="Tabela1" displayName="Tabela1" ref="A2:E28" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A2:E28" xr:uid="{FDB3D34F-B875-4993-9583-517C7A228CFA}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{118E91D1-00F1-42F6-9E02-866761859E49}" name="Step" dataDxfId="8" totalsRowDxfId="9">
+      <calculatedColumnFormula>Tabela2[[#Headers],[7. Use Device]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{B22BE939-BA72-4A25-ABE4-76EAAF8D34BF}" name="ID" dataDxfId="6" totalsRowDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{FDB88555-C521-4091-92DC-967EBE9E4630}" name="Name" dataDxfId="4" totalsRowDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{9387D76D-D771-4197-8E53-ECB36760E0F7}" name="User Story" dataDxfId="2" totalsRowDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{9A4DB8F3-E42F-4AEF-9F37-B344488A0BDC}" name="Acceptance Criteria" dataDxfId="0" totalsRowDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -972,18 +2010,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.44140625" customWidth="1"/>
-    <col min="3" max="3" width="35.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.109375" customWidth="1"/>
+    <col min="1" max="1" width="52.33203125" customWidth="1"/>
+    <col min="2" max="2" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35.88671875" customWidth="1"/>
     <col min="6" max="6" width="36.88671875" customWidth="1"/>
     <col min="7" max="7" width="35.5546875" customWidth="1"/>
@@ -995,25 +2033,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="H1" s="8" t="s">
         <v>31</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -1021,25 +2059,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -1047,13 +2085,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>5</v>
@@ -1062,10 +2100,10 @@
         <v>7</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -1074,78 +2112,921 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
-        <v>8</v>
+        <v>96</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11" t="s">
-        <v>23</v>
+        <v>97</v>
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="13"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>41</v>
-      </c>
+      <c r="A15" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="D16" s="27" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="D17" s="27" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="31"/>
+      <c r="C20" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="D20" s="33"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA0969E9-71A2-496D-8AD3-8391D2D4C914}">
+  <dimension ref="A1:E41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C12" zoomScale="87" workbookViewId="0">
+      <selection activeCell="D16" sqref="D14:D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="44.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" style="16" customWidth="1"/>
+    <col min="3" max="3" width="112.44140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="113" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41" style="16" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="78" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="20" t="str">
+        <f>Tabela2[[#Headers],[1. Unpack The Device]]</f>
+        <v>1. Unpack The Device</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="20" t="str">
+        <f>'Features from steps'!B2</f>
+        <v>1.1 Qr code on the device</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="20" t="str">
+        <f>Tabela2[[#Headers],[1. Unpack The Device]]</f>
+        <v>1. Unpack The Device</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="20" t="str">
+        <f>'Features from steps'!B3</f>
+        <v>1.2 Instruction manual in the box</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="20" t="str">
+        <f>Tabela2[[#Headers],[2. Open App]]</f>
+        <v>2. Open App</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="20" t="str">
+        <f>'Features from steps'!C2</f>
+        <v>2.1 Clickable App icon on mobile phone</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="20" t="str">
+        <f>Tabela2[[#Headers],[2. Open App]]</f>
+        <v>2. Open App</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="20" t="str">
+        <f>'Features from steps'!C3</f>
+        <v>2.2 Main app screen</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="20" t="str">
+        <f>Tabela2[[#Headers],[2. Open App]]</f>
+        <v>2. Open App</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="20" t="str">
+        <f>'Features from steps'!C4</f>
+        <v>2.3 "Add device" button</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A8" s="21" t="str">
+        <f>Tabela2[[#Headers],[2. Open App]]</f>
+        <v>2. Open App</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="20" t="str">
+        <f>'Features from steps'!C5</f>
+        <v>2.4 Item list screen</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="21" t="str">
+        <f>Tabela2[[#Headers],[2. Open App]]</f>
+        <v>2. Open App</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="20" t="str">
+        <f>'Features from steps'!C6</f>
+        <v>2.5 Bottom menu</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="20" t="str">
+        <f>Tabela2[[#Headers],[3. Scan QR Code]]</f>
+        <v>3. Scan QR Code</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="20" t="str">
+        <f>'Features from steps'!D2</f>
+        <v>3.1 Camera scanner</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="20" t="str">
+        <f>Tabela2[[#Headers],[3. Scan QR Code]]</f>
+        <v>3. Scan QR Code</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="20" t="str">
+        <f>'Features from steps'!D3</f>
+        <v>3.2 QR Detector</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="20" t="str">
+        <f>Tabela2[[#Headers],[3. Scan QR Code]]</f>
+        <v>3. Scan QR Code</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="20" t="str">
+        <f>'Features from steps'!D4</f>
+        <v>3.3 Scan feedback</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="20" t="str">
+        <f>Tabela2[[#Headers],[3. Scan QR Code]]</f>
+        <v>3. Scan QR Code</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="20" t="str">
+        <f>'Features from steps'!D5</f>
+        <v>3.4 Loading spinner</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="17" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="22" t="str">
+        <f>Tabela2[[#Headers],[4. Secure Pairing]]</f>
+        <v>4. Secure Pairing</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" s="22" t="str">
+        <f>'Features from steps'!E2</f>
+        <v>4.1 Run secure key exchange</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="22" t="str">
+        <f>Tabela2[[#Headers],[4. Secure Pairing]]</f>
+        <v>4. Secure Pairing</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="22" t="str">
+        <f>'Features from steps'!E3</f>
+        <v>4.2 Establish encrypted communication</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="22" t="str">
+        <f>Tabela2[[#Headers],[4. Secure Pairing]]</f>
+        <v>4. Secure Pairing</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="C16" s="22" t="str">
+        <f>'Features from steps'!E4</f>
+        <v>4.3 Retry pairing if needed</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="20" t="str">
+        <f>Tabela2[[#Headers],[5. See Connection]]</f>
+        <v>5. See Connection</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="20" t="str">
+        <f>'Features from steps'!F2</f>
+        <v>5.1 Success confirmation</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="20" t="str">
+        <f>Tabela2[[#Headers],[5. See Connection]]</f>
+        <v>5. See Connection</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="20" t="str">
+        <f>'Features from steps'!F3</f>
+        <v>5.2 Add device to device map</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="20" t="str">
+        <f>Tabela2[[#Headers],[5. See Connection]]</f>
+        <v>5. See Connection</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="20" t="str">
+        <f>'Features from steps'!F4</f>
+        <v>5.3 Show current status</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="20" t="str">
+        <f>Tabela2[[#Headers],[5. See Connection]]</f>
+        <v>5. See Connection</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="C20" s="20" t="str">
+        <f>'Features from steps'!F5</f>
+        <v>5.4 Load basic device profile</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A21" s="20" t="str">
+        <f>Tabela2[[#Headers],[5. See Connection]]</f>
+        <v>5. See Connection</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="C21" s="20" t="str">
+        <f>'Features from steps'!F6</f>
+        <v>5.5 Load advanced device profile</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="20" t="str">
+        <f>Tabela2[[#Headers],[6. Security Note]]</f>
+        <v>6. Security Note</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="20" t="str">
+        <f>'Features from steps'!G2</f>
+        <v>6.1 Security information pop-up</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="20" t="str">
+        <f>Tabela2[[#Headers],[6. Security Note]]</f>
+        <v>6. Security Note</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="20" t="str">
+        <f>'Features from steps'!G3</f>
+        <v>6.2 Secure defaults</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="20" t="str">
+        <f>Tabela2[[#Headers],[6. Security Note]]</f>
+        <v>6. Security Note</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="20" t="str">
+        <f>'Features from steps'!G4</f>
+        <v>6.3 Allow advanced security view</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="20" t="str">
+        <f>Tabela2[[#Headers],[7. Use Device]]</f>
+        <v>7. Use Device</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" s="20" t="str">
+        <f>'Features from steps'!H2</f>
+        <v>7.1 Connect/disconnect device</v>
+      </c>
+      <c r="D25" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="20" t="str">
+        <f>Tabela2[[#Headers],[7. Use Device]]</f>
+        <v>7. Use Device</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" s="20" t="str">
+        <f>'Features from steps'!H3</f>
+        <v>7.2 Show connection status</v>
+      </c>
+      <c r="D26" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A27" s="20" t="str">
+        <f>Tabela2[[#Headers],[7. Use Device]]</f>
+        <v>7. Use Device</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" s="20" t="str">
+        <f>'Features from steps'!H4</f>
+        <v>7.3 Basic security settings</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="E27" s="21" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="20" t="str">
+        <f>Tabela2[[#Headers],[7. Use Device]]</f>
+        <v>7. Use Device</v>
+      </c>
+      <c r="B28" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" s="20" t="str">
+        <f>'Features from steps'!H5</f>
+        <v>7.4 Advanced security settings</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="E28" s="21" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="34" t="str">
+        <f>Tabela3[[#Headers],[10. Set up device bluetooth]]</f>
+        <v>10. Set up device bluetooth</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="C29" s="22" t="str">
+        <f>'Features from steps'!B16</f>
+        <v>10.1 Import device bluetooth settings</v>
+      </c>
+      <c r="D29" s="22"/>
+      <c r="E29" s="23" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="34" t="str">
+        <f>Tabela3[[#Headers],[10. Set up device bluetooth]]</f>
+        <v>10. Set up device bluetooth</v>
+      </c>
+      <c r="B30" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="C30" s="22" t="str">
+        <f>'Features from steps'!B17</f>
+        <v>10.2 Set up beacon</v>
+      </c>
+      <c r="D30" s="35"/>
+      <c r="E30" s="36" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A31" s="34" t="str">
+        <f>Tabela3[[#Headers],[10. Set up device bluetooth]]</f>
+        <v>10. Set up device bluetooth</v>
+      </c>
+      <c r="B31" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="C31" s="22" t="str">
+        <f>'Features from steps'!B18</f>
+        <v>10.3 Connection to mobile phone HomeGuard app</v>
+      </c>
+      <c r="D31" s="35"/>
+      <c r="E31" s="36" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A32" s="34" t="str">
+        <f>Tabela3[[#Headers],[10. Set up device bluetooth]]</f>
+        <v>10. Set up device bluetooth</v>
+      </c>
+      <c r="B32" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="C32" s="22" t="str">
+        <f>'Features from steps'!B19</f>
+        <v>10.4 Energy management protocol</v>
+      </c>
+      <c r="D32" s="35"/>
+      <c r="E32" s="36" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A33" s="35" t="str">
+        <f>Tabela3[[#Headers],[11. Exchange protocol keys]]</f>
+        <v>11. Exchange protocol keys</v>
+      </c>
+      <c r="B33" s="35" t="s">
+        <v>141</v>
+      </c>
+      <c r="C33" s="35" t="str">
+        <f>'Features from steps'!C16</f>
+        <v>11.1 Generate keys based on device ID</v>
+      </c>
+      <c r="D33" s="35"/>
+      <c r="E33" s="36" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="35" t="str">
+        <f>Tabela3[[#Headers],[11. Exchange protocol keys]]</f>
+        <v>11. Exchange protocol keys</v>
+      </c>
+      <c r="B34" s="35" t="s">
+        <v>143</v>
+      </c>
+      <c r="C34" s="35" t="str">
+        <f>'Features from steps'!C17</f>
+        <v>11.2 Send public keys to mobile phone application using bluetooth connection</v>
+      </c>
+      <c r="D34" s="35"/>
+      <c r="E34" s="36" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="35" t="str">
+        <f>Tabela3[[#Headers],[11. Exchange protocol keys]]</f>
+        <v>11. Exchange protocol keys</v>
+      </c>
+      <c r="B35" s="35" t="s">
+        <v>144</v>
+      </c>
+      <c r="C35" s="35" t="str">
+        <f>'Features from steps'!C18</f>
+        <v>11.3 Receive session key</v>
+      </c>
+      <c r="D35" s="35"/>
+      <c r="E35" s="36" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A36" s="35" t="str">
+        <f>Tabela3[[#Headers],[11. Exchange protocol keys]]</f>
+        <v>11. Exchange protocol keys</v>
+      </c>
+      <c r="B36" s="35" t="s">
+        <v>145</v>
+      </c>
+      <c r="C36" s="35" t="str">
+        <f>'Features from steps'!C19</f>
+        <v>11.4 Differentiate keys between different connection types</v>
+      </c>
+      <c r="D36" s="35"/>
+      <c r="E36" s="36" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A37" s="35" t="str">
+        <f>Tabela3[[#Headers],[11. Exchange protocol keys]]</f>
+        <v>11. Exchange protocol keys</v>
+      </c>
+      <c r="B37" s="35" t="s">
+        <v>146</v>
+      </c>
+      <c r="C37" s="35" t="str">
+        <f>'Features from steps'!C20</f>
+        <v>11.5 Send different keys based on connection type</v>
+      </c>
+      <c r="D37" s="35"/>
+      <c r="E37" s="36" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A38" s="35" t="str">
+        <f>Tabela3[[#Headers],[12. Exchange data and establish secure connection]]</f>
+        <v>12. Exchange data and establish secure connection</v>
+      </c>
+      <c r="B38" s="35" t="s">
+        <v>142</v>
+      </c>
+      <c r="C38" s="35" t="str">
+        <f>'Features from steps'!D16</f>
+        <v>12.1 Ensure keys exchange</v>
+      </c>
+      <c r="D38" s="35"/>
+      <c r="E38" s="36" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="35" t="str">
+        <f>Tabela3[[#Headers],[12. Exchange data and establish secure connection]]</f>
+        <v>12. Exchange data and establish secure connection</v>
+      </c>
+      <c r="B39" s="35" t="s">
+        <v>147</v>
+      </c>
+      <c r="C39" s="35" t="str">
+        <f>'Features from steps'!D17</f>
+        <v>12.2 Exchange handshake</v>
+      </c>
+      <c r="D39" s="35"/>
+      <c r="E39" s="36" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="35" t="str">
+        <f>Tabela3[[#Headers],[12. Exchange data and establish secure connection]]</f>
+        <v>12. Exchange data and establish secure connection</v>
+      </c>
+      <c r="B40" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="C40" s="35" t="str">
+        <f>'Features from steps'!D18</f>
+        <v>12.4 Check for connection stability</v>
+      </c>
+      <c r="D40" s="35"/>
+      <c r="E40" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A41" s="35" t="str">
+        <f>Tabela3[[#Headers],[12. Exchange data and establish secure connection]]</f>
+        <v>12. Exchange data and establish secure connection</v>
+      </c>
+      <c r="B41" s="35" t="s">
+        <v>149</v>
+      </c>
+      <c r="C41" s="35" t="str">
+        <f>'Features from steps'!D19</f>
+        <v>12.5 Implement connection stability improvement algorithm</v>
+      </c>
+      <c r="D41" s="35"/>
+      <c r="E41" s="36" t="s">
+        <v>168</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>